<commit_message>
update host name for UAT1
</commit_message>
<xml_diff>
--- a/document/login_dp.xlsx
+++ b/document/login_dp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Dev2" sheetId="1" r:id="rId1"/>
@@ -1890,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>27</v>
@@ -2133,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update notes and document
</commit_message>
<xml_diff>
--- a/document/login_dp.xlsx
+++ b/document/login_dp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Dev2" sheetId="1" r:id="rId1"/>
@@ -1138,7 +1138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1444,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:I33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,9 +1790,12 @@
       <c r="A45" s="19"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="23" t="s">
         <v>113</v>
       </c>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
@@ -1837,7 +1840,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="A46:D46"/>
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="A23:I23"/>

</xml_diff>

<commit_message>
Add two Classes to verify differences between synchronized and Lock
</commit_message>
<xml_diff>
--- a/document/login_dp.xlsx
+++ b/document/login_dp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Dev2" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="152">
   <si>
     <t>Server Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -648,12 +648,19 @@
     <t>UAT1: http://diexp-uat.avnet.com/webapp/wcs/stores/servlet/en/ema</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/opt/ibm/was855_wp/profiles/wp_profile/logs/WebSphere_Portal/SystemOut.log</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -723,6 +730,12 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F497D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -762,7 +775,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -785,12 +798,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -819,6 +841,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -826,8 +850,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1536,7 +1560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A48" sqref="A48:D48"/>
     </sheetView>
   </sheetViews>
@@ -1694,17 +1718,17 @@
       <c r="D15" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
@@ -1718,30 +1742,30 @@
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
@@ -1755,56 +1779,56 @@
       <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
@@ -1818,59 +1842,59 @@
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -1893,12 +1917,12 @@
       <c r="D41" s="23"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
@@ -1907,12 +1931,12 @@
       <c r="D43" s="23"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
@@ -1921,12 +1945,12 @@
       <c r="D45" s="23"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="24" t="s">
+      <c r="A46" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
@@ -1935,19 +1959,19 @@
       <c r="D47" s="23"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="23"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1957,12 +1981,12 @@
       <c r="D50" s="23"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="s">
+      <c r="A51" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
@@ -1973,20 +1997,20 @@
       <c r="D52" s="23"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="26" t="s">
+      <c r="A59" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="28" t="s">
+      <c r="A60" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="27"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
@@ -2014,15 +2038,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A29:I29"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="A59:D59"/>
     <mergeCell ref="A60:D60"/>
@@ -2034,6 +2049,15 @@
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A29:I29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2057,10 +2081,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2068,9 +2092,10 @@
     <col min="1" max="2" width="12.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2083,8 +2108,11 @@
       <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="F1" s="31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>138</v>
       </c>
@@ -2097,8 +2125,11 @@
       <c r="D2" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="F2" s="32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>139</v>
       </c>

</xml_diff>

<commit_message>
update document by T430
</commit_message>
<xml_diff>
--- a/document/login_dp.xlsx
+++ b/document/login_dp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Dev2" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="151">
   <si>
     <t>Server Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -584,10 +584,6 @@
   </si>
   <si>
     <t>feb2017nick</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>aVn3t001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -843,6 +839,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -850,8 +848,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1254,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,7 +1386,7 @@
         <v>60</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1635,44 +1631,44 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6" s="17">
         <v>907729</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B7" s="17">
         <v>907729</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B8" s="17">
         <v>907729</v>
       </c>
       <c r="C8" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1718,17 +1714,17 @@
       <c r="D15" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
@@ -1742,30 +1738,30 @@
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
@@ -1779,56 +1775,56 @@
       <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
@@ -1842,59 +1838,59 @@
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -1917,12 +1913,12 @@
       <c r="D41" s="23"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
+      <c r="A42" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
@@ -1931,12 +1927,12 @@
       <c r="D43" s="23"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
@@ -1945,12 +1941,12 @@
       <c r="D45" s="23"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+      <c r="A46" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
@@ -1959,19 +1955,19 @@
       <c r="D47" s="23"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
+      <c r="A48" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
       <c r="D49" s="23"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1981,12 +1977,12 @@
       <c r="D50" s="23"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
@@ -1997,20 +1993,20 @@
       <c r="D52" s="23"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="28" t="s">
+      <c r="A59" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="B59" s="29"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="30" t="s">
+      <c r="A60" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
@@ -2038,15 +2034,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A29:I29"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="A59:D59"/>
     <mergeCell ref="A60:D60"/>
@@ -2058,6 +2045,15 @@
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A29:I29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2109,32 +2105,32 @@
         <v>3</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>44</v>
@@ -2676,7 +2672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
@@ -2920,7 +2916,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add sample code to check class initialization sequence
</commit_message>
<xml_diff>
--- a/document/login_dp.xlsx
+++ b/document/login_dp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Dev2" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="158">
   <si>
     <t>Server Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -673,6 +673,10 @@
   </si>
   <si>
     <t>may2017nick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jul2017nick</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1275,7 +1279,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,7 +1344,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2174,7 +2178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -2696,8 +2700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2734,7 +2738,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2748,7 +2752,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
create a new project for selenium
</commit_message>
<xml_diff>
--- a/document/login_dp.xlsx
+++ b/document/login_dp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Dev2" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="161">
   <si>
     <t>Server Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -694,6 +694,10 @@
   </si>
   <si>
     <t>sqlplus "A907729@(DESCRIPTION= (ADDRESS=(PROTOCOL=TCP)(HOST=venus-scan.avnet.com)(PORT=1521)) (CONNECT_DATA=(SERVER=DEDICATED) (SERVICE_NAME=avs93db.avnet.com)))"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sep2017nick</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -884,8 +888,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -893,6 +895,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1295,7 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1767,17 +1771,17 @@
       <c r="D15" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
@@ -1791,30 +1795,30 @@
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
@@ -1828,56 +1832,56 @@
       <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
@@ -1891,59 +1895,59 @@
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="27"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -1966,12 +1970,12 @@
       <c r="D41" s="23"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
@@ -1980,12 +1984,12 @@
       <c r="D43" s="23"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
+      <c r="A44" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
@@ -1994,12 +1998,12 @@
       <c r="D45" s="23"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
+      <c r="A46" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
@@ -2008,19 +2012,19 @@
       <c r="D47" s="23"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
+      <c r="A48" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
+      <c r="A49" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="23"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2030,12 +2034,12 @@
       <c r="D50" s="23"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
@@ -2046,20 +2050,20 @@
       <c r="D52" s="23"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="32" t="s">
+      <c r="A60" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
@@ -2087,6 +2091,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A29:I29"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="A59:D59"/>
     <mergeCell ref="A60:D60"/>
@@ -2098,15 +2111,6 @@
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A29:I29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2862,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2900,7 +2904,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
code for prog scala chapter3
</commit_message>
<xml_diff>
--- a/document/login_dp.xlsx
+++ b/document/login_dp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="761" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Dev2" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="163">
   <si>
     <t>Server Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -469,10 +469,6 @@
   </si>
   <si>
     <t>http://control.akaimai.com</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/opt/ibm/was70/profiles/appsrv/installedApps/adedv270cell/WC_emdi.ear/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -698,6 +694,18 @@
   </si>
   <si>
     <t>sep2017nick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Admin console</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tivoli02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/opt/ibm/was70/profiles/appsrv/installedApps/adedv270cell/WC_emdi.ear/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -888,6 +896,8 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -895,8 +905,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1242,7 +1250,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,7 +1264,7 @@
         <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" customFormat="1" ht="13.5" x14ac:dyDescent="0.15"/>
@@ -1285,7 +1293,7 @@
         <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1337,7 +1345,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1365,7 +1373,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1379,7 +1387,7 @@
         <v>44</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1393,7 +1401,7 @@
         <v>44</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1407,7 +1415,7 @@
         <v>44</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1435,7 +1443,7 @@
         <v>60</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1508,13 +1516,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1605,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:I21"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,58 +1688,58 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="17">
         <v>907729</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B7" s="17">
         <v>907729</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" s="17">
         <v>907729</v>
       </c>
       <c r="C8" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>133</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" s="17">
         <v>907729</v>
       </c>
       <c r="C9" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>145</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1741,9 +1749,15 @@
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
+      <c r="A11" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" s="17">
+        <v>913743</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>161</v>
+      </c>
       <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1771,17 +1785,17 @@
       <c r="D15" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17"/>
@@ -1795,30 +1809,30 @@
       <c r="I22" s="17"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
+      <c r="A23" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
+      <c r="A24" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
@@ -1832,56 +1846,56 @@
       <c r="I25" s="17"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
+      <c r="A28" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
+      <c r="A29" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
@@ -1895,59 +1909,59 @@
       <c r="I30" s="17"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="32"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -1970,12 +1984,12 @@
       <c r="D41" s="23"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
+      <c r="A42" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
@@ -1984,12 +1998,12 @@
       <c r="D43" s="23"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
+      <c r="A44" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
@@ -1998,12 +2012,12 @@
       <c r="D45" s="23"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
+      <c r="A46" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
@@ -2012,19 +2026,19 @@
       <c r="D47" s="23"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
+      <c r="A48" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="26" t="s">
+      <c r="A49" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
       <c r="D49" s="23"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2034,12 +2048,12 @@
       <c r="D50" s="23"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
@@ -2050,33 +2064,33 @@
       <c r="D52" s="23"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B59" s="29"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
+      <c r="A59" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
+      <c r="A60" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="B60" s="31"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B68" s="17">
         <v>907729</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2091,15 +2105,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A23:I23"/>
-    <mergeCell ref="A24:I24"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A29:I29"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="A59:D59"/>
     <mergeCell ref="A60:D60"/>
@@ -2111,6 +2116,15 @@
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A23:I23"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A29:I29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -2163,38 +2177,38 @@
         <v>3</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2246,7 +2260,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2260,7 +2274,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2288,7 +2302,7 @@
         <v>60</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2340,7 +2354,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2396,7 +2410,7 @@
         <v>46</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2447,7 +2461,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2461,7 +2475,7 @@
         <v>44</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2475,7 +2489,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2503,7 +2517,7 @@
         <v>46</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2554,7 +2568,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2568,7 +2582,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2582,7 +2596,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2610,7 +2624,7 @@
         <v>60</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2661,7 +2675,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2675,7 +2689,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2689,7 +2703,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2717,7 +2731,7 @@
         <v>60</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2768,7 +2782,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2782,7 +2796,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2852,7 +2866,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2866,7 +2880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2904,7 +2918,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2918,7 +2932,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2932,7 +2946,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2960,7 +2974,7 @@
         <v>46</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3011,7 +3025,7 @@
         <v>50</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3025,7 +3039,7 @@
         <v>50</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3039,7 +3053,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3109,7 +3123,7 @@
         <v>60</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>